<commit_message>
Committing the changes done in the tests to run them on IE 11.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_DeleteButtonDisabledInGF_WithEvidence.xlsx
+++ b/src/main/resources/testdata/Check_DeleteButtonDisabledInGF_WithEvidence.xlsx
@@ -530,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>

</xml_diff>